<commit_message>
Add basic query logic
</commit_message>
<xml_diff>
--- a/CSEnrolments.xlsx
+++ b/CSEnrolments.xlsx
@@ -4,13 +4,15 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9660" windowHeight="5490" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9660" windowHeight="5490"/>
   </bookViews>
   <sheets>
     <sheet name="CS206" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet2" sheetId="3" r:id="rId3"/>
     <sheet name="Sheet3" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet4" sheetId="5" r:id="rId5"/>
+    <sheet name="Sheet5" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
@@ -595,7 +597,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E37"/>
   <sheetViews>
-    <sheetView showRuler="0" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" showRuler="0" zoomScaleNormal="100" workbookViewId="0">
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
@@ -1086,7 +1088,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
@@ -1106,4 +1108,28 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add Loading for Students
</commit_message>
<xml_diff>
--- a/CSEnrolments.xlsx
+++ b/CSEnrolments.xlsx
@@ -13,28 +13,14 @@
   </bookViews>
   <sheets>
     <sheet name="CS206" sheetId="1" r:id="rId1"/>
+    <sheet name="CS204" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="80">
-  <si>
-    <t>Registration Number</t>
-  </si>
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Sessional Marks</t>
-  </si>
-  <si>
-    <t>End Semester Marks</t>
-  </si>
-  <si>
-    <t>Enrollment Status</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="87">
   <si>
     <t>cs121031</t>
   </si>
@@ -259,6 +245,42 @@
   </si>
   <si>
     <t>Junaid Yousuf Hamza</t>
+  </si>
+  <si>
+    <t>cs666666</t>
+  </si>
+  <si>
+    <t>cs666661</t>
+  </si>
+  <si>
+    <t>cs666662</t>
+  </si>
+  <si>
+    <t>cs666663</t>
+  </si>
+  <si>
+    <t>cs666664</t>
+  </si>
+  <si>
+    <t>cs666665</t>
+  </si>
+  <si>
+    <t>Student6</t>
+  </si>
+  <si>
+    <t>Student1</t>
+  </si>
+  <si>
+    <t>Student2</t>
+  </si>
+  <si>
+    <t>Student3</t>
+  </si>
+  <si>
+    <t>Student4</t>
+  </si>
+  <si>
+    <t>Student5</t>
   </si>
 </sst>
 </file>
@@ -598,10 +620,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E37"/>
+  <dimension ref="A1:E36"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -620,410 +642,393 @@
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
       <c r="E1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" t="s">
         <v>5</v>
-      </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E3" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E4" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E5" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B6" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E6" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E7" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B8" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E8" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B9" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E9" t="s">
-        <v>23</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B10" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E10" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B11" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E11" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B12" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E12" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B13" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="E13" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B14" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E14" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B15" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E15" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B16" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E16" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B17" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="E17" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B18" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E18" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B19" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E19" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B20" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E20" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B21" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="E21" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B22" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E22" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B23" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E23" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B24" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="E24" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E25" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B26" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E26" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B27" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="E27" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B28" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E28" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B29" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E29" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B30" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E30" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B31" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="E31" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B32" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E32" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B33" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E33" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B34" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E34" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B35" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E35" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B36" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="E36" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>78</v>
-      </c>
-      <c r="B37" t="s">
-        <v>79</v>
-      </c>
-      <c r="E37" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -1032,4 +1037,102 @@
   <pageSetup orientation="portrait"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="26.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>78</v>
+      </c>
+      <c r="B4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>79</v>
+      </c>
+      <c r="B8" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>80</v>
+      </c>
+      <c r="B9" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add Lots of Queries
</commit_message>
<xml_diff>
--- a/CSEnrolments.xlsx
+++ b/CSEnrolments.xlsx
@@ -9,18 +9,19 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9660" windowHeight="5490"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9660" windowHeight="5490" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="CS206" sheetId="1" r:id="rId1"/>
-    <sheet name="CS204" sheetId="2" r:id="rId2"/>
+    <sheet name="CS201" sheetId="3" r:id="rId2"/>
+    <sheet name="CS204" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="95">
   <si>
     <t>cs121031</t>
   </si>
@@ -281,6 +282,30 @@
   </si>
   <si>
     <t>Student5</t>
+  </si>
+  <si>
+    <t>Student7</t>
+  </si>
+  <si>
+    <t>Student8</t>
+  </si>
+  <si>
+    <t>Student9</t>
+  </si>
+  <si>
+    <t>Student10</t>
+  </si>
+  <si>
+    <t>cs666667</t>
+  </si>
+  <si>
+    <t>cs666677</t>
+  </si>
+  <si>
+    <t>cs666672</t>
+  </si>
+  <si>
+    <t>cs666673</t>
   </si>
 </sst>
 </file>
@@ -622,7 +647,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E36"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showRuler="0" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
@@ -1041,10 +1066,84 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="24.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B3" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>94</v>
+      </c>
+      <c r="B4" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Add Controller and functions for Handler
</commit_message>
<xml_diff>
--- a/CSEnrolments.xlsx
+++ b/CSEnrolments.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="97">
   <si>
     <t>cs121031</t>
   </si>
@@ -306,6 +306,12 @@
   </si>
   <si>
     <t>cs666673</t>
+  </si>
+  <si>
+    <t>cs777777</t>
+  </si>
+  <si>
+    <t>huyyy</t>
   </si>
 </sst>
 </file>
@@ -647,7 +653,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E36"/>
   <sheetViews>
-    <sheetView showRuler="0" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showRuler="0" topLeftCell="A20" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
@@ -1066,10 +1072,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1131,6 +1137,14 @@
       </c>
       <c r="B7" t="s">
         <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>95</v>
+      </c>
+      <c r="B8" t="s">
+        <v>96</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add View Home Scene
</commit_message>
<xml_diff>
--- a/CSEnrolments.xlsx
+++ b/CSEnrolments.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="95">
   <si>
     <t>cs121031</t>
   </si>
@@ -306,12 +306,6 @@
   </si>
   <si>
     <t>cs666673</t>
-  </si>
-  <si>
-    <t>cs777777</t>
-  </si>
-  <si>
-    <t>huyyy</t>
   </si>
 </sst>
 </file>
@@ -1072,10 +1066,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="A8" sqref="A8:XFD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1137,14 +1131,6 @@
       </c>
       <c r="B7" t="s">
         <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>95</v>
-      </c>
-      <c r="B8" t="s">
-        <v>96</v>
       </c>
     </row>
   </sheetData>

</xml_diff>